<commit_message>
updated yml file in all services
</commit_message>
<xml_diff>
--- a/Backend/tsp-user-service/src/test/resources/managers-tagging.xlsx
+++ b/Backend/tsp-user-service/src/test/resources/managers-tagging.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikku\Desktop\tsp\new-start\tsp-user-service\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahuly\Downloads\Talent-share-Portal-Application\Backend\tsp-user-service\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B1B066-1213-4810-9570-3A1CB840C26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18197229-44A7-4C5A-9FA7-4A276792C0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,44 +41,43 @@
     <t>rajesh</t>
   </si>
   <si>
-    <t>rajesh@maveric-systems.com</t>
-  </si>
-  <si>
     <t>srini</t>
   </si>
   <si>
-    <t>srini@maveric-systems.com</t>
-  </si>
-  <si>
     <t>praveen</t>
   </si>
   <si>
-    <t>praveen@maveric-systems.com</t>
-  </si>
-  <si>
     <t>vineet</t>
   </si>
   <si>
-    <t>vineet@maveric-systems.com</t>
-  </si>
-  <si>
     <t>prakash</t>
   </si>
   <si>
-    <t>prakash@maveric-systems.com</t>
-  </si>
-  <si>
     <t>daisy</t>
   </si>
   <si>
-    <t>daisy@maveric-systems.com</t>
+    <t>rajesh@gmail.com</t>
+  </si>
+  <si>
+    <t>srini@gmail.com</t>
+  </si>
+  <si>
+    <t>praveen@gmail.com</t>
+  </si>
+  <si>
+    <t>vineet@gmail.com</t>
+  </si>
+  <si>
+    <t>prakash@gmail.com</t>
+  </si>
+  <si>
+    <t>daisy@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,16 +443,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.90625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="29.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -478,61 +477,61 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>

</xml_diff>